<commit_message>
Updated import method to disallow null values for mandatory fields
</commit_message>
<xml_diff>
--- a/iCare/resources/sample1.xlsx
+++ b/iCare/resources/sample1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafiz\Documents\UofT\4th Year\1st Semester\CSCC01\Project\Team22\iCare\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6617D68B-C8F1-4C6A-9175-6CD2E3BD8F52}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5C63DB58-D104-4A53-975D-99FBDDFD7476}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{C6A3135D-C732-472C-B9D8-A19BA277115A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>hello</t>
   </si>
@@ -43,6 +43,21 @@
   </si>
   <si>
     <t>heading</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>Bye</t>
+  </si>
+  <si>
+    <t>Cya</t>
+  </si>
+  <si>
+    <t>Lol</t>
+  </si>
+  <si>
+    <t>Why</t>
   </si>
 </sst>
 </file>
@@ -394,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D36BA158-3147-48CE-B2F6-69B3F4212731}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,20 +440,54 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>44</v>
+      </c>
+      <c r="E5">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed import method to deal with null cells
</commit_message>
<xml_diff>
--- a/iCare/resources/sample1.xlsx
+++ b/iCare/resources/sample1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafiz\Documents\UofT\4th Year\1st Semester\CSCC01\Project\Team22\iCare\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6617D68B-C8F1-4C6A-9175-6CD2E3BD8F52}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{75204F9B-3A1C-4313-B553-CEDC4BEDC07F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{C6A3135D-C732-472C-B9D8-A19BA277115A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>hello</t>
   </si>
@@ -43,6 +43,21 @@
   </si>
   <si>
     <t>heading</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>Bye</t>
+  </si>
+  <si>
+    <t>Cya</t>
+  </si>
+  <si>
+    <t>Lol</t>
+  </si>
+  <si>
+    <t>Why</t>
   </si>
 </sst>
 </file>
@@ -394,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D36BA158-3147-48CE-B2F6-69B3F4212731}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,20 +440,54 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <v>4</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>44</v>
+      </c>
+      <c r="E5">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated and tested import with mandatory fields missing/filled, etc
</commit_message>
<xml_diff>
--- a/iCare/resources/sample1.xlsx
+++ b/iCare/resources/sample1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafiz\Documents\UofT\4th Year\1st Semester\CSCC01\Project\Team22\iCare\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5C63DB58-D104-4A53-975D-99FBDDFD7476}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5FFC6A29-0544-408B-BBD1-4883399284CD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{C6A3135D-C732-472C-B9D8-A19BA277115A}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,13 +72,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -93,8 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +434,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,19 +462,19 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated sample files for testing
</commit_message>
<xml_diff>
--- a/iCare/resources/sample1.xlsx
+++ b/iCare/resources/sample1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hafiz\Documents\UofT\4th Year\1st Semester\CSCC01\Project\Team22\iCare\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{75204F9B-3A1C-4313-B553-CEDC4BEDC07F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5FFC6A29-0544-408B-BBD1-4883399284CD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{C6A3135D-C732-472C-B9D8-A19BA277115A}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,13 +72,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -93,8 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +434,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,19 +462,19 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>